<commit_message>
dealt with the carbon flows, cleaned the sankey code and plot
</commit_message>
<xml_diff>
--- a/data/aldo_clc_categories.xlsx
+++ b/data/aldo_clc_categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bohnenkl\Documents\GitHub\silvia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADA6811-53F7-459F-8366-3DB3F7E98A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF39C7F-9CBD-4F27-B12A-4972F951EA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED05BED7-5647-43CF-BCB7-6C64B278C0C2}"/>
   </bookViews>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42B01C4-F636-487B-A8F7-3AB7E65725D1}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1367,6 +1367,9 @@
       <c r="D17" t="s">
         <v>5</v>
       </c>
+      <c r="E17" s="37">
+        <v>313</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1583,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>45</v>

</xml_diff>